<commit_message>
Implementacion de interaccion para cerrar ventanas modales ocasionales no controladas
</commit_message>
<xml_diff>
--- a/src/test/resources/data/AlojamientoSeleccionado.xlsx
+++ b/src/test/resources/data/AlojamientoSeleccionado.xlsx
@@ -23,13 +23,13 @@
     <t>Precio</t>
   </si>
   <si>
-    <t>I Loft You - Hermoso apartamento en Medellín</t>
+    <t>Apartamento tipo Ático, piso 4 SIN Ascensor</t>
   </si>
   <si>
-    <t>Carolina</t>
+    <t>Hey You</t>
   </si>
   <si>
-    <t>$1,225,760.93 COP</t>
+    <t>$1,022,861.32 COP</t>
   </si>
 </sst>
 </file>
@@ -80,7 +80,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="40.55859375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="8.96484375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.1015625" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>

<commit_message>
Actualizacion de dependencias en el gradle a la misma version
</commit_message>
<xml_diff>
--- a/src/test/resources/data/AlojamientoSeleccionado.xlsx
+++ b/src/test/resources/data/AlojamientoSeleccionado.xlsx
@@ -23,13 +23,13 @@
     <t>Precio</t>
   </si>
   <si>
-    <t>Apartamento tipo Ático, piso 4 SIN Ascensor</t>
+    <t>I Loft You - Hermoso apartamento en Medellín</t>
   </si>
   <si>
-    <t>Hey You</t>
+    <t>Carolina</t>
   </si>
   <si>
-    <t>$1,022,861.32 COP</t>
+    <t>$1,221,457.68 COP</t>
   </si>
 </sst>
 </file>
@@ -80,7 +80,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.55859375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="42.671875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="8.96484375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.1015625" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>